<commit_message>
updated the second test case
</commit_message>
<xml_diff>
--- a/tests/test_data_sheet.xlsx
+++ b/tests/test_data_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pandiaraj\library_management\apps\library_management_system\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE176B33-20F0-45C8-B71B-C208A53315EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9CE4B8-2929-4489-A3F3-DD8611869D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Login Successful</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>TC_002</t>
   </si>
   <si>
@@ -101,44 +104,56 @@
     <t>Test Login Screen with useremail and password should not be empty</t>
   </si>
   <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Date of Joining</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>TC-0001</t>
   </si>
   <si>
     <t>To verify the valid members data</t>
   </si>
   <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Date of Joining</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Kathir</t>
   </si>
   <si>
     <t>kathir.s@gmail.com</t>
   </si>
   <si>
-    <t>Activate</t>
-  </si>
-  <si>
-    <t>Member Added</t>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Saved</t>
+  </si>
+  <si>
+    <t>This is member already added.</t>
+  </si>
+  <si>
+    <t>TC-0002</t>
+  </si>
+  <si>
+    <t>Test the Existing Member Email ID Should not be Allowed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +165,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,7 +200,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
@@ -476,7 +497,7 @@
     <col min="5" max="6" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -515,67 +536,70 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>12344456789</v>
@@ -584,24 +608,24 @@
         <v>5677</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -617,11 +641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405F0092-B17C-460B-A189-7569A553CB4F}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,7 +655,7 @@
     <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -645,19 +669,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -668,16 +692,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>8956234578</v>
@@ -686,15 +710,46 @@
         <v>45962</v>
       </c>
       <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E3">
+        <v>8956234578</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45962</v>
+      </c>
+      <c r="G3" t="s">
         <v>36</v>
       </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{80D05E96-761F-4CA0-B10F-48A6B66A5C19}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{32E07A94-B463-47FC-BEA7-BB110FB7A5D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>